<commit_message>
R vs Python 3, 4, 5
</commit_message>
<xml_diff>
--- a/Wechat Working Record.xlsx
+++ b/Wechat Working Record.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cxin\Documents\Wechat-\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8980" yWindow="280" windowWidth="25600" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8976" yWindow="276" windowWidth="25596" windowHeight="15564" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Paper Review" sheetId="1" r:id="rId1"/>
     <sheet name="R vs Python" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t xml:space="preserve">R </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,24 +103,42 @@
   <si>
     <t>By</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>pd.sort_value</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>read.csv</t>
+  </si>
+  <si>
+    <t>pd.read_csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -124,7 +147,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -133,7 +156,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -141,7 +164,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -181,14 +204,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -518,7 +549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -532,19 +563,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="21.296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.796875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.796875" style="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -591,45 +622,73 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>